<commit_message>
commit on 22 july  2019
</commit_message>
<xml_diff>
--- a/src/test/java/com/nmc/api/testdata/Locators.xlsx
+++ b/src/test/java/com/nmc/api/testdata/Locators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="486">
   <si>
     <t xml:space="preserve">Web Element Name</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t xml:space="preserve">patientContactNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id or name(pre-reg)</t>
   </si>
   <si>
     <t xml:space="preserve">patient_care_oftext</t>
@@ -1170,6 +1173,312 @@
   </si>
   <si>
     <t xml:space="preserve">d_diagnosis_status_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Locators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchDropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//span[text()="Search"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activePatientLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linkText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Patients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientSearchLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patients Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visitSearchLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visits Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableRow0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//tr[@id='toolbarRow0']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editPatientDetailsLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toolbarTitleDiv_defaultPatientEdit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration Success locator for Validation in regInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//fieldset[@id="regInfo"]/table[1]/tbody[1]/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientVisitId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[2]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[3]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consultingDepartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[4]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consultingDoctor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[5]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseFileNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[6]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[7]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tokenNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="regInfo"]/table/tbody/tr[8]/td[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BillingDropDown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//span[contains(text(),'Billing')] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientVisitIdTextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="ps_visit"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FindButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@value="Find"]       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchBillLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Bills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finalizeBedCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_finalze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saveButtonForFinalizeBedCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">childBirthLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">babyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateOfBirth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeOfBirth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">babyAttendingDepartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">babyAttendingDeptIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doctorName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bedtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">childBirthRemarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resetButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@type="reset"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PatientphysicalDischarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DischargeLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientVisitIdField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ps_visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@value="Find"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bed Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//a[text()='Bed Details']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="content"]/form[1]/table/tbody/tr[5]/td/a[4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billStatusDropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okToDischarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_okToDischarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okToDischargeDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dischargeDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billSaveButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saveButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DischargeStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="content"]/form[2]/fieldset/table/tbody/tr[1]/td[2]/b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TtypeOfDischarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discharge_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dethDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deathTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dethOnArrival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dead_on_arrival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deathReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death_reason_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discharge_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dischargeTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discharge_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dischargeDoctor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discharge_doc_ac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dischargeButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Finalize Locator</t>
   </si>
 </sst>
 </file>
@@ -1308,10 +1617,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K227"/>
+  <dimension ref="A1:K398"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A207" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D225" activeCellId="0" sqref="B224:D225"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A275" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B289" activeCellId="0" sqref="B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1455,6 +1764,9 @@
       <c r="B10" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="C10" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="0" t="s">
         <v>16</v>
       </c>
@@ -1723,10 +2035,10 @@
         <v>56</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,13 +2046,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,13 +2060,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,13 +2074,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,13 +2088,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,13 +2102,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,13 +2116,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,13 +2130,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,13 +2144,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,13 +2158,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,13 +2172,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,13 +2186,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,7 +2205,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,10 +2213,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,10 +2227,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,10 +2241,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,10 +2255,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,10 +2269,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,10 +2283,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1967,10 +2297,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,13 +2311,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,13 +2325,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,10 +2339,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,10 +2350,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,13 +2361,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,13 +2375,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,10 +2389,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,10 +2400,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,13 +2411,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,10 +2425,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,10 +2436,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2114,10 +2447,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,10 +2458,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,13 +2469,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,13 +2483,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,10 +2497,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,10 +2508,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,10 +2519,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,10 +2530,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,10 +2541,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,10 +2552,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2568,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,10 +2576,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,10 +2587,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,7 +2603,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,10 +2611,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,10 +2622,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,13 +2633,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,13 +2647,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,13 +2661,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2342,13 +2675,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,13 +2689,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,13 +2703,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,10 +2717,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2395,10 +2728,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2406,10 +2739,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2417,13 +2750,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,13 +2764,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,13 +2778,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,13 +2792,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,13 +2806,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,13 +2820,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2501,13 +2834,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,13 +2848,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,13 +2862,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,13 +2876,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,13 +2890,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,13 +2904,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,13 +2918,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,13 +2932,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2613,13 +2946,13 @@
         <v>103</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,13 +2960,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2641,13 +2974,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2993,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,13 +3001,13 @@
         <v>108</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,13 +3015,13 @@
         <v>109</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,13 +3029,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,13 +3043,13 @@
         <v>111</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,13 +3057,13 @@
         <v>112</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2738,13 +3071,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,13 +3085,13 @@
         <v>114</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2766,13 +3099,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2780,13 +3113,13 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,13 +3127,13 @@
         <v>117</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,13 +3141,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2822,13 +3155,13 @@
         <v>119</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,13 +3169,13 @@
         <v>120</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,13 +3183,13 @@
         <v>121</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C122" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,13 +3197,13 @@
         <v>122</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2878,13 +3211,13 @@
         <v>123</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,13 +3225,13 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,13 +3239,13 @@
         <v>125</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2920,13 +3253,13 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2934,13 +3267,13 @@
         <v>127</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,13 +3281,13 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C129" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,13 +3295,13 @@
         <v>129</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C130" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,7 +3314,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,13 +3322,13 @@
         <v>132</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3003,13 +3336,13 @@
         <v>133</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,7 +3355,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,13 +3363,13 @@
         <v>136</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3044,13 +3377,13 @@
         <v>137</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,13 +3391,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C139" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,13 +3405,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3086,13 +3419,13 @@
         <v>140</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3100,13 +3433,13 @@
         <v>141</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,13 +3447,13 @@
         <v>142</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C143" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3128,13 +3461,13 @@
         <v>143</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,13 +3475,13 @@
         <v>144</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C145" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3156,13 +3489,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C146" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3170,13 +3503,13 @@
         <v>146</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3189,7 +3522,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,13 +3530,13 @@
         <v>149</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C150" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,13 +3544,13 @@
         <v>150</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C151" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,13 +3558,13 @@
         <v>151</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C152" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,13 +3572,13 @@
         <v>152</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C153" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,13 +3586,13 @@
         <v>153</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C154" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,13 +3600,13 @@
         <v>154</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C155" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3281,13 +3614,13 @@
         <v>155</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C156" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,7 +3633,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3308,13 +3641,13 @@
         <v>158</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C159" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3327,7 +3660,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3335,13 +3668,13 @@
         <v>161</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C162" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,13 +3682,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C163" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,13 +3696,13 @@
         <v>163</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C164" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3377,13 +3710,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C165" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,10 +3724,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,13 +3735,13 @@
         <v>166</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C167" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,13 +3749,13 @@
         <v>167</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C168" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,13 +3763,13 @@
         <v>168</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C169" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3444,13 +3777,13 @@
         <v>169</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C170" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,7 +3796,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3471,7 +3804,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,13 +3812,13 @@
         <v>173</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,10 +3826,10 @@
         <v>174</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3504,13 +3837,13 @@
         <v>175</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C176" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,13 +3851,13 @@
         <v>176</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C177" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3532,13 +3865,13 @@
         <v>177</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C178" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,13 +3879,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C179" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,13 +3893,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C180" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3574,10 +3907,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,10 +3918,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,13 +3929,13 @@
         <v>182</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C183" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,10 +3943,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3621,10 +3954,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3632,10 +3965,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3643,10 +3976,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3654,13 +3987,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,7 +4001,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3676,13 +4009,13 @@
         <v>189</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C190" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3690,13 +4023,13 @@
         <v>190</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C191" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,13 +4037,13 @@
         <v>191</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C192" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3718,13 +4051,13 @@
         <v>192</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C193" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3737,7 +4070,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3745,13 +4078,13 @@
         <v>195</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C196" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3759,13 +4092,13 @@
         <v>196</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C197" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,13 +4106,13 @@
         <v>197</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C198" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,13 +4120,13 @@
         <v>198</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C199" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3811,10 +4144,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3827,10 +4163,10 @@
         <v>203</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3838,10 +4174,10 @@
         <v>204</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,10 +4185,10 @@
         <v>205</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3860,10 +4196,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3871,13 +4207,13 @@
         <v>207</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C208" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3885,13 +4221,13 @@
         <v>208</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C209" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,7 +4260,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3932,13 +4268,13 @@
         <v>215</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3946,13 +4282,13 @@
         <v>216</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3960,13 +4296,13 @@
         <v>217</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C218" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3974,13 +4310,13 @@
         <v>218</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3988,13 +4324,13 @@
         <v>219</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4017,7 +4353,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,13 +4361,13 @@
         <v>224</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4042,6 +4378,1344 @@
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="3" t="n">
         <v>226</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="3" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="3" t="n">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="3" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="3" t="n">
+        <v>230</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="3" t="n">
+        <v>231</v>
+      </c>
+      <c r="B232" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C232" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D232" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="3" t="n">
+        <v>232</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D233" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="3" t="n">
+        <v>233</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C234" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D234" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="3" t="n">
+        <v>234</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="C235" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="3" t="n">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="3" t="n">
+        <v>236</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="3" t="n">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="3" t="n">
+        <v>238</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C239" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D239" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="3" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="3" t="n">
+        <v>240</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="3" t="n">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="3" t="n">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="3" t="n">
+        <v>243</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="3" t="n">
+        <v>244</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D245" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="3" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D246" s="0" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="3" t="n">
+        <v>246</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D247" s="0" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="3" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D248" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="3" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D249" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="3" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D250" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="3" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D251" s="0" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="3" t="n">
+        <v>251</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C252" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D252" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="3" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="3" t="n">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="3" t="n">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="3" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="3" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="3" t="n">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="3" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="3" t="n">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="3" t="n">
+        <v>260</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C261" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D261" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="3" t="n">
+        <v>261</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D262" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="3" t="n">
+        <v>262</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D263" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="3" t="n">
+        <v>263</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="C264" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D264" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="3" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="3" t="n">
+        <v>265</v>
+      </c>
+      <c r="B266" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="C266" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D266" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="3" t="n">
+        <v>266</v>
+      </c>
+      <c r="B267" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C267" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D267" s="0" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="3" t="n">
+        <v>267</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="C268" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D268" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="3" t="n">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="3" t="n">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="3" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="3" t="n">
+        <v>271</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="3" t="n">
+        <v>272</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C273" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D273" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="3" t="n">
+        <v>273</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="D274" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="3" t="n">
+        <v>274</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="D275" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="3" t="n">
+        <v>275</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D276" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="3" t="n">
+        <v>276</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="D277" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="3" t="n">
+        <v>277</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D278" s="0" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="3" t="n">
+        <v>278</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="D279" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="3" t="n">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="3" t="n">
+        <v>280</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="D281" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="3" t="n">
+        <v>281</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="D282" s="0" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="3" t="n">
+        <v>282</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D283" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="3" t="n">
+        <v>283</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D284" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="3" t="n">
+        <v>284</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D285" s="0" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="3" t="n">
+        <v>285</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D286" s="0" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="3" t="n">
+        <v>286</v>
+      </c>
+      <c r="B287" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D287" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="3" t="n">
+        <v>287</v>
+      </c>
+      <c r="B288" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="D288" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="3" t="n">
+        <v>288</v>
+      </c>
+      <c r="B289" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="C289" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D289" s="0" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="3" t="n">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="3" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="3" t="n">
+        <v>291</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="3" t="n">
+        <v>292</v>
+      </c>
+      <c r="B293" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="C293" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D293" s="0" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="3" t="n">
+        <v>293</v>
+      </c>
+      <c r="B294" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C294" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D294" s="0" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="3" t="n">
+        <v>294</v>
+      </c>
+      <c r="B295" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="D295" s="0" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="3" t="n">
+        <v>295</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="C296" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D296" s="0" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="3" t="n">
+        <v>296</v>
+      </c>
+      <c r="B297" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="C297" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D297" s="0" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="3" t="n">
+        <v>297</v>
+      </c>
+      <c r="B298" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D298" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="3" t="n">
+        <v>298</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C299" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D299" s="0" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="3" t="n">
+        <v>299</v>
+      </c>
+      <c r="B300" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C300" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D300" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="3" t="n">
+        <v>300</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="C301" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D301" s="0" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="3" t="n">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="3" t="n">
+        <v>302</v>
+      </c>
+      <c r="B303" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D303" s="0" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="3" t="n">
+        <v>303</v>
+      </c>
+      <c r="B304" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C304" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D304" s="0" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="3" t="n">
+        <v>304</v>
+      </c>
+      <c r="B305" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D305" s="0" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="3" t="n">
+        <v>305</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D306" s="0" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="3" t="n">
+        <v>306</v>
+      </c>
+      <c r="B307" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C307" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D307" s="0" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="3" t="n">
+        <v>307</v>
+      </c>
+      <c r="B308" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C308" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D308" s="0" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="3" t="n">
+        <v>308</v>
+      </c>
+      <c r="B309" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D309" s="0" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="3" t="n">
+        <v>309</v>
+      </c>
+      <c r="B310" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D310" s="0" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="3" t="n">
+        <v>310</v>
+      </c>
+      <c r="B311" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="D311" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="3" t="n">
+        <v>311</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="C312" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D312" s="0" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="3" t="n">
+        <v>312</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="3" t="n">
+        <v>313</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="3" t="n">
+        <v>314</v>
+      </c>
+      <c r="B315" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="3" t="n">
+        <v>315</v>
+      </c>
+      <c r="B316" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="3" t="n">
+        <v>316</v>
+      </c>
+      <c r="B317" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="3" t="n">
+        <v>317</v>
+      </c>
+      <c r="B318" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="3" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="3" t="n">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="3" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="3" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="3" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="3" t="n">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="3" t="n">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="3" t="n">
+        <v>325</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="3" t="n">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="3" t="n">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="3" t="n">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="3" t="n">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="3" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="3" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="3" t="n">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="3" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="3" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="3" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="3" t="n">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="3" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="3" t="n">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="3" t="n">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="3" t="n">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="3" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="3" t="n">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="3" t="n">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="3" t="n">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="3" t="n">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="3" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="3" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="3" t="n">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="3" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="3" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="3" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="3" t="n">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="3" t="n">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="3" t="n">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="3" t="n">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="3" t="n">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="3" t="n">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="3" t="n">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="3" t="n">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="3" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="3" t="n">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="3" t="n">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="3" t="n">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="3" t="n">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="3" t="n">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="3" t="n">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="3" t="n">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="3" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="3" t="n">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="3" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="3" t="n">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="3" t="n">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="3" t="n">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="3" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="3" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="3" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="3" t="n">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="3" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="3" t="n">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="3" t="n">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="3" t="n">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="3" t="n">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="3" t="n">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="3" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="3" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="3" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="3" t="n">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="3" t="n">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="3" t="n">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="3" t="n">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="3" t="n">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="3" t="n">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="3" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="3" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="3" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="3" t="n">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="3" t="n">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>